<commit_message>
Remove files (security issues)
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Caminhos e URLs para arquivos" sheetId="1" r:id="rId1"/>
     <sheet name="Nomes das colunas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
   <si>
     <t>Caminhos e URLs para abrir informações, ou baixá-las quando não estiverem disponíveis fisicamente</t>
   </si>
@@ -54,9 +53,6 @@
     <t>URL para tabela preenchida na base</t>
   </si>
   <si>
-    <t>https://onedrive.live.com/download.aspx?cid=0c5702aadd8306c5&amp;page=view&amp;resid=C5702AADD8306C5!6977&amp;parId=C5702AADD8306C5!1072&amp;app=Excel</t>
-  </si>
-  <si>
     <t>Caminho físico para o arquivo da tabela dos formulários</t>
   </si>
   <si>
@@ -64,9 +60,6 @@
   </si>
   <si>
     <t>URL para o arquivo da tabela dos formulários</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/spreadsheets/d/1_iu8HSeeTIRPI3ENQkQY4QCWXzIdJQBVJhy6w9USHGI/export?format=xlsx</t>
   </si>
   <si>
     <t>Informações Gerais</t>
@@ -1137,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1175,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1183,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,25 +1214,21 @@
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="str">
@@ -1247,7 +1236,7 @@
         <v>Nome da aba das informações gerais em Forms.xlsx</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1256,7 +1245,7 @@
         <v>Nome da aba das informações da vítima em Forms.xlsx</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1254,7 @@
         <v>Nome da aba das informações do veículo em Forms.xlsx</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1274,17 +1263,13 @@
         <v>Nome da aba das informações de balística Forms.xlsx</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1294,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1314,92 +1299,92 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="42"/>
       <c r="G1" s="42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="42"/>
       <c r="K1" s="42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="D3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="E3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
@@ -1408,124 +1393,124 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="G4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="33" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="E5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="F5" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="G5" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="E6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="F6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="G6" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="H6" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="D7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="F7" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="G7" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="H7" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="E8" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="F8" s="40" t="s">
         <v>65</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>67</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="35"/>
@@ -1533,16 +1518,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>70</v>
-      </c>
       <c r="D9" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
@@ -1552,74 +1537,74 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="D10" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1631,86 +1616,86 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>